<commit_message>
Ya casi al 100
Hace integrales múltiples indefinidas, integrales simples definidas, permite regresar al primer entry el resultado, valida las iteraciones y recibe varias variables. Aún se ve algo feito, faltan acomodar cosas, y falta que los datos se muestren con formato (de preferencia)
</commit_message>
<xml_diff>
--- a/Matemáticas Registro.xlsx
+++ b/Matemáticas Registro.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Semana 6</t>
   </si>
@@ -37,6 +37,12 @@
     <t>Semana 12</t>
   </si>
   <si>
+    <t>Semana 13</t>
+  </si>
+  <si>
+    <t>Semana 14</t>
+  </si>
+  <si>
     <t>Juárez Escamilla Guadalupe Montserrat</t>
   </si>
   <si>
@@ -46,6 +52,15 @@
     <t>Documentación</t>
   </si>
   <si>
+    <t>Correción de fallos</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>ps en curso</t>
+  </si>
+  <si>
     <t>Loeza García Luis Arturo</t>
   </si>
   <si>
@@ -58,10 +73,28 @@
     <t>Programación Visual</t>
   </si>
   <si>
+    <t>Correción de fallas</t>
+  </si>
+  <si>
+    <t>Verificación Tkinter</t>
+  </si>
+  <si>
+    <t>Ps en curso</t>
+  </si>
+  <si>
     <t>Vega Ledesma Axel Francisco</t>
   </si>
   <si>
     <t>Programación Lógica</t>
+  </si>
+  <si>
+    <t>Lógica</t>
+  </si>
+  <si>
+    <t>Corrección de fallas</t>
+  </si>
+  <si>
+    <t>Verificaciones Sympy</t>
   </si>
 </sst>
 </file>
@@ -85,13 +118,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFffffff"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFffffff"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -153,31 +186,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,21 +523,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="6.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="21.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="22.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="24.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="8" width="22.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="22.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="3.4335714285714283" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="17.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="17.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="15.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="15.576428571428572" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="8" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="23.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="12.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="10" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="11" width="18.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="1">
@@ -508,94 +552,138 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="33" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="63" customFormat="1" s="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="33" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="69.75" customFormat="1" s="1">
       <c r="A4" s="3"/>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="B4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="33.75" customFormat="1" s="1">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="58.5" customFormat="1" s="1">
       <c r="A5" s="3"/>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>